<commit_message>
[docs] update static analysis v0.0.1 result
update static analysis v0.0.1 result
</commit_message>
<xml_diff>
--- a/docs/09_static_analysis/static_analysis_20210608_v0.0.1_reviewed.xlsx
+++ b/docs/09_static_analysis/static_analysis_20210608_v0.0.1_reviewed.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\cmu_project\docs\09_static_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\09_static_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,18 +13,19 @@
   </bookViews>
   <sheets>
     <sheet name="cppchecker_20210608_v0.0.1" sheetId="1" r:id="rId1"/>
-    <sheet name="flawfinder_20210607_v0.0.1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="flawfinder_20210607_v0.0.1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cppchecker_20210608_v0.0.1'!$C$1:$C$155</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">flawfinder_20210607_v0.0.1!$B$1:$B$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">flawfinder_20210607_v0.0.1!$B$1:$B$125</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="296">
   <si>
     <t>File</t>
   </si>
@@ -966,6 +967,10 @@
   </si>
   <si>
     <t>cmu_project\source\LgFaceRecDemoTCP_Jetson_NanoV2\MTCNN_FaceDetection_TensorRT\src\common.cpp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1589,7 +1594,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1603,6 +1608,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1662,6 +1670,1242 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'cppchecker_20210608_v0.0.1'!$H$162</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>number</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'cppchecker_20210608_v0.0.1'!$G$163:$G$178</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>constParameter</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ctuOneDefinitionRuleViolation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>invalidPointerCast</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>missingOverride</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>noCopyConstructor</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>noExplicitConstructor</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>noOperatorEq</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>passedByValue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>postfixOperator</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>uninitMemberVar</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>unreadVariable</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>unsignedLessThanZero</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unusedFunction</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>unusedLabel</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>useInitializationList</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>variableScope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'cppchecker_20210608_v0.0.1'!$H$163:$H$178</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2171700</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="차트 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1927,10 +3171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J159"/>
+  <dimension ref="A1:J178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5140,14 +6384,189 @@
         <v>289</v>
       </c>
     </row>
+    <row r="162" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G162" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H162" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="163" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G163" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H163" s="5">
+        <f>COUNTIF(F2:F155,G163)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G164" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H164" s="5">
+        <f t="shared" ref="H164:H178" si="0">COUNTIF(F3:F156,G164)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G165" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H165" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G166" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H166" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G167" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H167" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G168" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H168" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G169" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H169" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G170" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H170" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G171" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H171" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G172" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H172" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="173" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G173" t="s">
+        <v>15</v>
+      </c>
+      <c r="H173" s="5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="174" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G174" t="s">
+        <v>22</v>
+      </c>
+      <c r="H174" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G175" t="s">
+        <v>18</v>
+      </c>
+      <c r="H175" s="5">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="176" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G176" t="s">
+        <v>110</v>
+      </c>
+      <c r="H176" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G177" t="s">
+        <v>103</v>
+      </c>
+      <c r="H177" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G178" t="s">
+        <v>9</v>
+      </c>
+      <c r="H178" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="C1:C155"/>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <sortState ref="A1:A159">
+    <sortCondition ref="A1:A159"/>
+  </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S130"/>
   <sheetViews>

</xml_diff>